<commit_message>
Add Soyuz and Proton-M rocket families + updated launh parameters
</commit_message>
<xml_diff>
--- a/Real Solar System/RSS - Launch Parameters.xlsx
+++ b/Real Solar System/RSS - Launch Parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Vessel Name</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Apoapsis</t>
   </si>
   <si>
-    <t>Inclination</t>
-  </si>
-  <si>
     <t>Turn Altitude[km]</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Launch Site</t>
-  </si>
-  <si>
     <t>Falcon 9 FT</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>Kerbitat 3,75m - Recycler</t>
   </si>
   <si>
-    <t>Baikonur</t>
-  </si>
-  <si>
     <t>SLS-Block1B Crew</t>
   </si>
   <si>
@@ -159,13 +150,10 @@
     <t>Omega [rad/s]</t>
   </si>
   <si>
-    <t>Proton-K</t>
-  </si>
-  <si>
-    <t>Soyuz-FG</t>
-  </si>
-  <si>
-    <t>Stop at stage 3</t>
+    <t>Soyuz Family</t>
+  </si>
+  <si>
+    <t>Proton-M Family</t>
   </si>
 </sst>
 </file>
@@ -633,28 +621,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,278 +652,257 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>375</v>
       </c>
-      <c r="C2">
-        <v>56.1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="C2" s="3">
         <v>0.25</v>
       </c>
-      <c r="F2">
+      <c r="D2">
         <v>50</v>
       </c>
+      <c r="E2">
+        <v>165</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
       <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>375</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>165</v>
+      </c>
+      <c r="F3" s="3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+      <c r="I3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>265</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
         <v>180</v>
       </c>
-      <c r="H2" s="3">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>40</v>
-      </c>
-      <c r="J2">
+      <c r="F4" s="3">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>41</v>
+      </c>
+      <c r="H4">
         <v>90</v>
       </c>
-      <c r="K2">
+      <c r="I4">
         <v>90</v>
       </c>
-      <c r="L2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>265</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
-      </c>
-      <c r="G3">
-        <v>180</v>
-      </c>
-      <c r="H3" s="3">
-        <v>13</v>
-      </c>
-      <c r="I3">
-        <v>41</v>
-      </c>
-      <c r="J3">
-        <v>90</v>
-      </c>
-      <c r="K3">
-        <v>90</v>
-      </c>
-      <c r="L3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4">
-        <v>375</v>
-      </c>
-      <c r="C4">
-        <v>51.6</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4">
-        <v>180</v>
-      </c>
-      <c r="H4" s="3">
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="I4">
-        <v>40</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="B5">
         <v>355</v>
       </c>
-      <c r="E5" s="3">
+      <c r="C5" s="3">
         <v>0.25</v>
       </c>
-      <c r="F5">
+      <c r="D5">
         <v>50</v>
       </c>
+      <c r="E5">
+        <v>180</v>
+      </c>
+      <c r="F5" s="3">
+        <v>13</v>
+      </c>
       <c r="G5">
-        <v>180</v>
-      </c>
-      <c r="H5" s="3">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
       </c>
       <c r="I5">
-        <v>40</v>
-      </c>
-      <c r="J5">
         <v>90</v>
       </c>
-      <c r="K5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>355</v>
       </c>
-      <c r="E6" s="3">
+      <c r="C6" s="3">
         <v>0.25</v>
       </c>
-      <c r="F6">
+      <c r="D6">
         <v>50</v>
       </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6" s="3">
+        <v>11</v>
+      </c>
       <c r="G6">
-        <v>180</v>
-      </c>
-      <c r="H6" s="3">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>90</v>
       </c>
       <c r="I6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J6">
-        <v>90</v>
-      </c>
-      <c r="K6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B7">
         <v>275</v>
       </c>
-      <c r="E7" s="3">
+      <c r="C7" s="3">
         <v>0.25</v>
       </c>
-      <c r="F7">
+      <c r="D7">
         <v>50</v>
       </c>
+      <c r="E7">
+        <v>180</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
       <c r="G7">
-        <v>180</v>
-      </c>
-      <c r="H7" s="3">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>40</v>
-      </c>
-      <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>275</v>
       </c>
-      <c r="E8" s="3">
+      <c r="C8" s="3">
         <v>0.25</v>
       </c>
-      <c r="F8">
+      <c r="D8">
         <v>50</v>
       </c>
+      <c r="E8">
+        <v>180</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
       <c r="G8">
-        <v>180</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>90</v>
       </c>
       <c r="I8">
-        <v>36</v>
-      </c>
-      <c r="J8">
         <v>90</v>
       </c>
-      <c r="K8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>403</v>
       </c>
-      <c r="E9" s="3">
+      <c r="C9" s="3">
         <v>0.25</v>
       </c>
-      <c r="F9">
+      <c r="D9">
         <v>10</v>
       </c>
+      <c r="E9">
+        <v>180</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-10</v>
+      </c>
       <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9">
         <v>180</v>
       </c>
-      <c r="H9" s="3">
-        <v>-10</v>
-      </c>
       <c r="I9">
-        <v>45</v>
-      </c>
-      <c r="J9">
-        <v>180</v>
-      </c>
-      <c r="K9">
         <v>180</v>
       </c>
     </row>
@@ -970,12 +936,12 @@
     <row r="1" spans="1:23" ht="15.75" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4">
         <v>-1.4666666666666599</v>
@@ -983,7 +949,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4">
         <v>-0.97333333333333305</v>
@@ -991,7 +957,7 @@
     </row>
     <row r="4" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>-148.048</v>
@@ -1016,7 +982,7 @@
     </row>
     <row r="5" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>-1224</v>
@@ -1024,7 +990,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" thickTop="1">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
         <v>0.133333333333333</v>
@@ -1032,7 +998,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4">
         <v>1.2266666666666599</v>
@@ -1040,7 +1006,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>127.906666666666</v>
@@ -1048,48 +1014,48 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="R11" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>37</v>
@@ -1166,7 +1132,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>138</v>
@@ -1255,13 +1221,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="11">
         <v>5.9700000000000003E+24</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="11">
         <v>6.67E-11</v>
@@ -1269,7 +1235,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="10">
         <v>6378137</v>
@@ -1277,17 +1243,17 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickTop="1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="10">
         <v>270</v>
@@ -1299,7 +1265,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="12">
         <f xml:space="preserve"> 0.001*(POWER($F$1*$B$1/$C$6/$C$6,1/3)-$B$2)</f>
@@ -1308,7 +1274,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="12">
         <f>C6*($B$2 + 1000*$B$7)</f>

</xml_diff>

<commit_message>
Update launch parameters with Space Shuttle options
</commit_message>
<xml_diff>
--- a/Real Solar System/RSS - Launch Parameters.xlsx
+++ b/Real Solar System/RSS - Launch Parameters.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,10 +734,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B4">
-        <v>265</v>
+        <v>375</v>
       </c>
       <c r="C4" s="3">
         <v>0.25</v>
@@ -746,27 +746,27 @@
         <v>50</v>
       </c>
       <c r="E4">
+        <v>165</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
         <v>180</v>
       </c>
-      <c r="F4" s="3">
-        <v>13</v>
-      </c>
-      <c r="G4">
-        <v>41</v>
-      </c>
-      <c r="H4">
-        <v>90</v>
-      </c>
       <c r="I4">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>355</v>
+        <v>265</v>
       </c>
       <c r="C5" s="3">
         <v>0.25</v>
@@ -781,7 +781,7 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5">
         <v>90</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>355</v>
@@ -807,10 +807,10 @@
         <v>180</v>
       </c>
       <c r="F6" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>90</v>
@@ -821,10 +821,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="C7" s="3">
         <v>0.25</v>
@@ -836,21 +836,21 @@
         <v>180</v>
       </c>
       <c r="F7" s="3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>275</v>
@@ -865,45 +865,45 @@
         <v>180</v>
       </c>
       <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>40</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>36</v>
-      </c>
-      <c r="H8">
-        <v>90</v>
-      </c>
       <c r="I8">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>403</v>
+        <v>275</v>
       </c>
       <c r="C9" s="3">
         <v>0.25</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>180</v>
       </c>
       <c r="F9" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H9">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="I9">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor adjustments for Space Shuttle & SRB-4
</commit_message>
<xml_diff>
--- a/Real Solar System/RSS - Launch Parameters.xlsx
+++ b/Real Solar System/RSS - Launch Parameters.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -749,7 +749,7 @@
         <v>165</v>
       </c>
       <c r="F4" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>40</v>

</xml_diff>

<commit_message>
Adjust lauch parameters for Saturn V
</commit_message>
<xml_diff>
--- a/Real Solar System/RSS - Launch Parameters.xlsx
+++ b/Real Solar System/RSS - Launch Parameters.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,7 +682,7 @@
         <v>375</v>
       </c>
       <c r="C2" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -711,7 +711,7 @@
         <v>375</v>
       </c>
       <c r="C3" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -740,7 +740,7 @@
         <v>375</v>
       </c>
       <c r="C4" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -769,7 +769,7 @@
         <v>265</v>
       </c>
       <c r="C5" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -778,10 +778,10 @@
         <v>180</v>
       </c>
       <c r="F5" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>90</v>
@@ -798,7 +798,7 @@
         <v>355</v>
       </c>
       <c r="C6" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -827,7 +827,7 @@
         <v>355</v>
       </c>
       <c r="C7" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -856,7 +856,7 @@
         <v>275</v>
       </c>
       <c r="C8" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -885,7 +885,7 @@
         <v>275</v>
       </c>
       <c r="C9" s="3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
         <v>50</v>

</xml_diff>